<commit_message>
researching inline nav for About page
</commit_message>
<xml_diff>
--- a/New Features implementation plan-2020.xlsx
+++ b/New Features implementation plan-2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Igor Houwat - Branding - Alumni\Branding Tactics\Promotion\PRL Website\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4A7A69-EC11-4D60-809E-35660D9FD0CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C21558F-7730-4F4E-8FB4-2AEFB92E1067}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>Feature</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Scrolling nav</t>
-  </si>
-  <si>
     <t>Explore Zoom timelines</t>
   </si>
   <si>
@@ -135,6 +132,15 @@
   </si>
   <si>
     <t>Publish</t>
+  </si>
+  <si>
+    <t>Time spent</t>
+  </si>
+  <si>
+    <t>25 minutes</t>
+  </si>
+  <si>
+    <t>Research mobile applications; determine PRL-appropriate structure; maybe ask Federica for opinion</t>
   </si>
 </sst>
 </file>
@@ -189,7 +195,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -207,13 +216,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{18181141-9763-4C4E-81E2-BD8C4A1BC2B5}" name="Table1" displayName="Table1" ref="A1:D31" totalsRowShown="0">
-  <autoFilter ref="A1:D31" xr:uid="{9D8E2DD3-3A32-40AB-A43D-21CD0663BC75}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{18181141-9763-4C4E-81E2-BD8C4A1BC2B5}" name="Table1" displayName="Table1" ref="A1:E31" totalsRowShown="0">
+  <autoFilter ref="A1:E31" xr:uid="{9D8E2DD3-3A32-40AB-A43D-21CD0663BC75}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{7F3EECCF-1821-47EC-B71B-035ADD8DACD4}" name="Feature"/>
-    <tableColumn id="2" xr3:uid="{5FAB022F-5EFF-4925-8EBB-2E122BE73721}" name="Tasks" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{5FAB022F-5EFF-4925-8EBB-2E122BE73721}" name="Tasks" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{8FFB4A38-2812-4604-85EC-33574A58F8A9}" name="Time Cost (in hours)"/>
-    <tableColumn id="4" xr3:uid="{93DF2C04-3550-4F5A-8C44-5008FCE2F361}" name="Notes"/>
+    <tableColumn id="5" xr3:uid="{26D05208-6FB9-41CD-BB6D-843F20FE28C0}" name="Time spent"/>
+    <tableColumn id="4" xr3:uid="{93DF2C04-3550-4F5A-8C44-5008FCE2F361}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -482,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -493,10 +503,11 @@
     <col min="1" max="1" width="21.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.08984375" customWidth="1"/>
+    <col min="5" max="5" width="32.36328125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -507,16 +518,19 @@
         <v>10</v>
       </c>
       <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
@@ -524,10 +538,13 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
@@ -535,7 +552,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
@@ -543,15 +560,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
@@ -559,13 +576,13 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
@@ -573,7 +590,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
@@ -581,176 +598,176 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12">
         <v>3</v>
       </c>
-      <c r="D12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E12" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13">
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14">
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B15" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16">
         <v>1.5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C25">
         <v>1.5</v>
       </c>
-      <c r="D25" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E25" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>8</v>
       </c>
       <c r="B27" s="2"/>
     </row>
-    <row r="28" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B28" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C28">
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B30" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="C29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B30" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31">

</xml_diff>

<commit_message>
updated research on inline nav
</commit_message>
<xml_diff>
--- a/New Features implementation plan-2020.xlsx
+++ b/New Features implementation plan-2020.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Igor Houwat - Branding - Alumni\Branding Tactics\Promotion\PRL Website\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C21558F-7730-4F4E-8FB4-2AEFB92E1067}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56F17CF-46F0-42CD-8901-A6740B504B40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -137,17 +137,37 @@
     <t>Time spent</t>
   </si>
   <si>
-    <t>25 minutes</t>
-  </si>
-  <si>
-    <t>Research mobile applications; determine PRL-appropriate structure; maybe ask Federica for opinion</t>
+    <t>50 minutes</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Research mobile applications;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> determine PRL-appropriate structure; maybe ask Federica for opinion</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +177,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -495,7 +523,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -549,7 +577,7 @@
         <v>11</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -772,7 +800,7 @@
       <c r="B31" s="2"/>
       <c r="C31">
         <f>SUM(C2:C30)</f>
-        <v>37.75</v>
+        <v>38.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Researching About page inpage nav
</commit_message>
<xml_diff>
--- a/New Features implementation plan-2020.xlsx
+++ b/New Features implementation plan-2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Igor Houwat - Branding - Alumni\Branding Tactics\Promotion\PRL Website\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56F17CF-46F0-42CD-8901-A6740B504B40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B194DE6-0FA8-44E4-B6DB-8711BCBE0DE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -137,7 +137,7 @@
     <t>Time spent</t>
   </si>
   <si>
-    <t>50 minutes</t>
+    <t>1hr 5min</t>
   </si>
   <si>
     <r>
@@ -159,7 +159,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> determine PRL-appropriate structure; maybe ask Federica for opinion</t>
+      <t xml:space="preserve"> Determine PRL-appropriate structure; Design XD mockup; Maybe ask Federica for opinion</t>
     </r>
   </si>
 </sst>
@@ -523,7 +523,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -532,7 +532,7 @@
     <col min="2" max="2" width="20.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.08984375" customWidth="1"/>
-    <col min="5" max="5" width="32.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.1796875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added new feature to-do
</commit_message>
<xml_diff>
--- a/New Features implementation plan-2020.xlsx
+++ b/New Features implementation plan-2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Igor Houwat - Branding - Alumni\Branding Tactics\Promotion\PRL Website\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B194DE6-0FA8-44E4-B6DB-8711BCBE0DE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A46A61D-2B9C-4A14-8789-7A4887F39084}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>Feature</t>
   </si>
@@ -161,6 +161,21 @@
       </rPr>
       <t xml:space="preserve"> Determine PRL-appropriate structure; Design XD mockup; Maybe ask Federica for opinion</t>
     </r>
+  </si>
+  <si>
+    <t>News story progress bar</t>
+  </si>
+  <si>
+    <t>Research</t>
+  </si>
+  <si>
+    <t>Codepen design</t>
+  </si>
+  <si>
+    <t>Implement</t>
+  </si>
+  <si>
+    <t>Determine if needed at all</t>
   </si>
 </sst>
 </file>
@@ -244,8 +259,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{18181141-9763-4C4E-81E2-BD8C4A1BC2B5}" name="Table1" displayName="Table1" ref="A1:E31" totalsRowShown="0">
-  <autoFilter ref="A1:E31" xr:uid="{9D8E2DD3-3A32-40AB-A43D-21CD0663BC75}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{18181141-9763-4C4E-81E2-BD8C4A1BC2B5}" name="Table1" displayName="Table1" ref="A1:E36" totalsRowShown="0">
+  <autoFilter ref="A1:E36" xr:uid="{9D8E2DD3-3A32-40AB-A43D-21CD0663BC75}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{7F3EECCF-1821-47EC-B71B-035ADD8DACD4}" name="Feature"/>
     <tableColumn id="2" xr3:uid="{5FAB022F-5EFF-4925-8EBB-2E122BE73721}" name="Tasks" dataDxfId="1"/>
@@ -520,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -606,201 +621,247 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="C9">
-        <v>0.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C10">
-        <v>0.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="C12">
-        <v>3</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13">
-        <v>0.5</v>
-      </c>
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B14" s="2" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C14">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B15" s="2" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C17">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C18">
+      <c r="C23">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="1"/>
-      <c r="B21" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="1"/>
-      <c r="B23" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="1"/>
-      <c r="B24" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C25">
-        <v>1.5</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="1"/>
+      <c r="B27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="1"/>
+      <c r="B28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="1"/>
+      <c r="B29" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="1"/>
+      <c r="B30" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30">
+        <v>1.5</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="1"/>
+      <c r="B31" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C26">
+      <c r="C31">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="2"/>
-    </row>
-    <row r="28" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B28" s="2" t="s">
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="B33" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C28">
+      <c r="C33">
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B29" s="2" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B34" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B30" s="2" t="s">
+      <c r="C34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B35" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C30">
+      <c r="C35">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="3" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="2"/>
-      <c r="C31">
-        <f>SUM(C2:C30)</f>
-        <v>38.75</v>
+      <c r="B36" s="2"/>
+      <c r="C36">
+        <f>SUM(C2:C35)</f>
+        <v>47.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated new features plan
</commit_message>
<xml_diff>
--- a/New Features implementation plan-2020.xlsx
+++ b/New Features implementation plan-2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Igor Houwat - Branding - Alumni\Branding Tactics\Promotion\PRL Website\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A46A61D-2B9C-4A14-8789-7A4887F39084}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDF2C1C-126F-4AC2-BCD0-FC9889139677}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -137,7 +137,22 @@
     <t>Time spent</t>
   </si>
   <si>
-    <t>1hr 5min</t>
+    <t>News story progress bar</t>
+  </si>
+  <si>
+    <t>Research</t>
+  </si>
+  <si>
+    <t>Codepen design</t>
+  </si>
+  <si>
+    <t>Implement</t>
+  </si>
+  <si>
+    <t>Determine if needed at all</t>
+  </si>
+  <si>
+    <t>1hr 15min</t>
   </si>
   <si>
     <r>
@@ -149,7 +164,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Research mobile applications;</t>
+      <t>Research mobile applications; Ask Jesse for advice;</t>
     </r>
     <r>
       <rPr>
@@ -161,21 +176,6 @@
       </rPr>
       <t xml:space="preserve"> Determine PRL-appropriate structure; Design XD mockup; Maybe ask Federica for opinion</t>
     </r>
-  </si>
-  <si>
-    <t>News story progress bar</t>
-  </si>
-  <si>
-    <t>Research</t>
-  </si>
-  <si>
-    <t>Codepen design</t>
-  </si>
-  <si>
-    <t>Implement</t>
-  </si>
-  <si>
-    <t>Determine if needed at all</t>
   </si>
 </sst>
 </file>
@@ -538,7 +538,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" activeCellId="1" sqref="C3 B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -573,7 +573,7 @@
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
@@ -581,10 +581,10 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -621,21 +621,21 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -659,7 +659,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C12">
         <v>1</v>

</xml_diff>

<commit_message>
sticky nav: added markup
</commit_message>
<xml_diff>
--- a/New Features implementation plan-2020.xlsx
+++ b/New Features implementation plan-2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Igor Houwat - Branding - Alumni\Branding Tactics\Promotion\PRL Website\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466574BC-642C-4957-B820-9A9CB9E3F643}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58E50B3-F708-450B-8BD6-9F74841A2447}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>Feature</t>
   </si>
@@ -186,7 +186,13 @@
     </r>
   </si>
   <si>
-    <t>4hr</t>
+    <t>4hr15min</t>
+  </si>
+  <si>
+    <t>0.5hr</t>
+  </si>
+  <si>
+    <t>DONE Add &lt;h2&gt; with anchors; Style menu; JS autopopulate menu feature; Scroll between sections; NEW FORK: Tentative: inject aside with JS, inject anchors by scrubbing &lt;h2&gt; text nodes</t>
   </si>
 </sst>
 </file>
@@ -549,7 +555,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -558,7 +564,7 @@
     <col min="2" max="2" width="20.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.08984375" customWidth="1"/>
-    <col min="5" max="5" width="37.1796875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="39" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -598,12 +604,18 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -872,7 +884,7 @@
       <c r="B36" s="2"/>
       <c r="C36">
         <f>SUM(C2:C35)</f>
-        <v>47.75</v>
+        <v>48.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sticky nav: auto populate feature
</commit_message>
<xml_diff>
--- a/New Features implementation plan-2020.xlsx
+++ b/New Features implementation plan-2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Igor Houwat - Branding - Alumni\Branding Tactics\Promotion\PRL Website\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58E50B3-F708-450B-8BD6-9F74841A2447}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4502DD11-B263-4E91-BB32-B44F42C93CBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -189,10 +189,10 @@
     <t>4hr15min</t>
   </si>
   <si>
-    <t>0.5hr</t>
-  </si>
-  <si>
-    <t>DONE Add &lt;h2&gt; with anchors; Style menu; JS autopopulate menu feature; Scroll between sections; NEW FORK: Tentative: inject aside with JS, inject anchors by scrubbing &lt;h2&gt; text nodes</t>
+    <t>3hr45min</t>
+  </si>
+  <si>
+    <t>DONE Add &lt;h2&gt; with anchors; DONE Style menu; DONE JS autopopulate menu feature; Scroll between sections; NEW FORK: Tentative: inject aside with JS, inject anchors by scrubbing &lt;h2&gt; text nodes</t>
   </si>
 </sst>
 </file>
@@ -564,7 +564,7 @@
     <col min="2" max="2" width="20.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.08984375" customWidth="1"/>
-    <col min="5" max="5" width="39" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.6328125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -590,7 +590,7 @@
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
@@ -609,7 +609,7 @@
         <v>11</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
         <v>41</v>
@@ -884,7 +884,7 @@
       <c r="B36" s="2"/>
       <c r="C36">
         <f>SUM(C2:C35)</f>
-        <v>48.75</v>
+        <v>49.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding smooth scroll to side nav
</commit_message>
<xml_diff>
--- a/New Features implementation plan-2020.xlsx
+++ b/New Features implementation plan-2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Igor Houwat - Branding - Alumni\Branding Tactics\Promotion\PRL Website\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4502DD11-B263-4E91-BB32-B44F42C93CBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65ACB508-C797-412F-9567-0B9C7B5EC735}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -189,10 +189,10 @@
     <t>4hr15min</t>
   </si>
   <si>
-    <t>3hr45min</t>
-  </si>
-  <si>
     <t>DONE Add &lt;h2&gt; with anchors; DONE Style menu; DONE JS autopopulate menu feature; Scroll between sections; NEW FORK: Tentative: inject aside with JS, inject anchors by scrubbing &lt;h2&gt; text nodes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4hr </t>
   </si>
 </sst>
 </file>
@@ -555,7 +555,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -612,10 +612,10 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
accessibility: aria label and focus interactions
</commit_message>
<xml_diff>
--- a/New Features implementation plan-2020.xlsx
+++ b/New Features implementation plan-2020.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Igor Houwat - Branding - Alumni\Branding Tactics\Promotion\PRL Website\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65ACB508-C797-412F-9567-0B9C7B5EC735}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38896E2D-C172-4487-8D61-76A4880D1ABF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
   <si>
     <t>Feature</t>
   </si>
@@ -189,10 +189,13 @@
     <t>4hr15min</t>
   </si>
   <si>
-    <t>DONE Add &lt;h2&gt; with anchors; DONE Style menu; DONE JS autopopulate menu feature; Scroll between sections; NEW FORK: Tentative: inject aside with JS, inject anchors by scrubbing &lt;h2&gt; text nodes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4hr </t>
+    <t xml:space="preserve">8hr </t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>Upload to Code pen at this point</t>
   </si>
 </sst>
 </file>
@@ -244,13 +247,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -604,7 +610,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
@@ -612,10 +618,10 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -624,6 +630,12 @@
       </c>
       <c r="C5">
         <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1.75</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
adapted styles to PRL site / fixed UI bugs
</commit_message>
<xml_diff>
--- a/New Features implementation plan-2020.xlsx
+++ b/New Features implementation plan-2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Igor Houwat - Branding - Alumni\Branding Tactics\Promotion\PRL Website\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38896E2D-C172-4487-8D61-76A4880D1ABF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6405F72-5BC1-42E8-8925-D119008DECDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -561,7 +561,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -645,6 +645,9 @@
       <c r="C6">
         <v>2</v>
       </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">

</xml_diff>

<commit_message>
Implemented sticky side nav in production
</commit_message>
<xml_diff>
--- a/New Features implementation plan-2020.xlsx
+++ b/New Features implementation plan-2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Igor Houwat - Branding - Alumni\Branding Tactics\Promotion\PRL Website\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6405F72-5BC1-42E8-8925-D119008DECDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D20007E-A5DC-4749-8044-2249612669AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -195,7 +195,7 @@
     <t>DONE</t>
   </si>
   <si>
-    <t>Upload to Code pen at this point</t>
+    <t>Upload to Code pen at this point; extra time spent debugging on browsers…</t>
   </si>
 </sst>
 </file>
@@ -227,12 +227,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -247,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -257,6 +263,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,7 +568,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -624,7 +631,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
@@ -632,7 +639,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="4">
-        <v>1.75</v>
+        <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>43</v>
@@ -646,7 +653,7 @@
         <v>2</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -656,9 +663,12 @@
       <c r="C7">
         <v>0.5</v>
       </c>
+      <c r="D7">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B8" s="2" t="s">

</xml_diff>

<commit_message>
demo for article progress bar
</commit_message>
<xml_diff>
--- a/New Features implementation plan-2020.xlsx
+++ b/New Features implementation plan-2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Igor Houwat - Branding - Alumni\Branding Tactics\Promotion\PRL Website\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D20007E-A5DC-4749-8044-2249612669AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF3D56E-609F-457D-8AF9-29B2FB7AE3A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -141,9 +141,6 @@
   </si>
   <si>
     <t>Research</t>
-  </si>
-  <si>
-    <t>Codepen design</t>
   </si>
   <si>
     <t>Implement</t>
@@ -196,6 +193,9 @@
   </si>
   <si>
     <t>Upload to Code pen at this point; extra time spent debugging on browsers…</t>
+  </si>
+  <si>
+    <t>Design</t>
   </si>
 </sst>
 </file>
@@ -568,7 +568,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -611,10 +611,10 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -625,10 +625,10 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -642,7 +642,7 @@
         <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -677,15 +677,21 @@
       <c r="C8">
         <v>2</v>
       </c>
+      <c r="D8">
+        <v>0.5</v>
+      </c>
       <c r="E8" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
         <v>3</v>
       </c>
     </row>
@@ -696,6 +702,9 @@
       <c r="C10">
         <v>1</v>
       </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
@@ -707,7 +716,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12">
         <v>1</v>

</xml_diff>

<commit_message>
implemented progress bar in production
</commit_message>
<xml_diff>
--- a/New Features implementation plan-2020.xlsx
+++ b/New Features implementation plan-2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Igor Houwat - Branding - Alumni\Branding Tactics\Promotion\PRL Website\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF3D56E-609F-457D-8AF9-29B2FB7AE3A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA25D50D-DAB5-4B81-8E47-F1A44CA3BD87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>Feature</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>Design</t>
+  </si>
+  <si>
+    <t>Includes cross browser testing</t>
   </si>
 </sst>
 </file>
@@ -253,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -264,6 +267,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -568,7 +572,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -668,7 +672,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -713,6 +717,9 @@
       <c r="C11">
         <v>2</v>
       </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
@@ -721,9 +728,15 @@
       <c r="C12">
         <v>1</v>
       </c>
+      <c r="D12">
+        <v>0.5</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="A13" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="2"/>

</xml_diff>

<commit_message>
Updated About page and hero img styles
</commit_message>
<xml_diff>
--- a/New Features implementation plan-2020.xlsx
+++ b/New Features implementation plan-2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Igor Houwat - Branding - Alumni\Branding Tactics\Promotion\PRL Website\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA25D50D-DAB5-4B81-8E47-F1A44CA3BD87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE9ACAF-591B-47C3-A6E1-0283DCF44F98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>Feature</t>
   </si>
@@ -181,12 +181,6 @@
       </rPr>
       <t>Determine PRL-appropriate structure; Design XD mockup; Maybe ask Federica for opinion</t>
     </r>
-  </si>
-  <si>
-    <t>4hr15min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8hr </t>
   </si>
   <si>
     <t>DONE</t>
@@ -263,11 +257,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -614,8 +608,8 @@
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
-        <v>39</v>
+      <c r="D3">
+        <v>4.25</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>38</v>
@@ -628,11 +622,11 @@
       <c r="C4">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
-        <v>40</v>
+      <c r="D4">
+        <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -642,11 +636,11 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="6">
         <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -672,7 +666,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -690,7 +684,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -732,7 +726,7 @@
         <v>0.5</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -748,6 +742,9 @@
       <c r="C14">
         <v>0.5</v>
       </c>
+      <c r="D14">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B15" s="2" t="s">
@@ -756,9 +753,12 @@
       <c r="C15">
         <v>0.25</v>
       </c>
+      <c r="D15">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="A16" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="2"/>

</xml_diff>

<commit_message>
Added progress bar & sticky side menu to web components
</commit_message>
<xml_diff>
--- a/New Features implementation plan-2020.xlsx
+++ b/New Features implementation plan-2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Igor Houwat - Branding - Alumni\Branding Tactics\Promotion\PRL Website\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE9ACAF-591B-47C3-A6E1-0283DCF44F98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B27FDE-1FA1-4018-B444-688BFEDD9DD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>Feature</t>
   </si>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t>Notes</t>
-  </si>
-  <si>
-    <t>Explore Zoom timelines</t>
   </si>
   <si>
     <t>Touch base with Christoph</t>
@@ -194,6 +191,15 @@
   <si>
     <t>Includes cross browser testing</t>
   </si>
+  <si>
+    <t>Prepare but postpone application. Due to COVID, MSU is asking for iages of people with PPE</t>
+  </si>
+  <si>
+    <t>Research format</t>
+  </si>
+  <si>
+    <t>A Zoom Timeline is too clunky</t>
+  </si>
 </sst>
 </file>
 
@@ -224,7 +230,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -234,6 +240,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -250,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -261,6 +273,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -565,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -589,7 +604,7 @@
         <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>14</v>
@@ -612,7 +627,7 @@
         <v>4.25</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -626,7 +641,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -640,12 +655,12 @@
         <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -667,10 +682,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -679,12 +694,12 @@
         <v>0.5</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -706,7 +721,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -717,7 +732,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -726,7 +741,7 @@
         <v>0.5</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -765,26 +780,32 @@
     </row>
     <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17">
         <v>3</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B18" s="2" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="C18">
-        <v>0.5</v>
+        <v>1.25</v>
+      </c>
+      <c r="D18">
+        <v>0.75</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B19" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19">
         <v>1.5</v>
@@ -792,7 +813,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B20" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -800,7 +821,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B21" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C21">
         <v>1.5</v>
@@ -808,7 +829,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B22" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -816,7 +837,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B23" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -831,7 +852,7 @@
     <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C25">
         <v>4</v>
@@ -840,7 +861,7 @@
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26">
         <v>2</v>
@@ -849,7 +870,7 @@
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -858,7 +879,7 @@
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C28">
         <v>3</v>
@@ -867,7 +888,7 @@
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -876,33 +897,36 @@
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C30">
         <v>1.5</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C31">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>8</v>
       </c>
       <c r="B32" s="2"/>
+      <c r="E32" s="7" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="33" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="B33" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C33">
         <v>0.5</v>
@@ -910,7 +934,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B34" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C34">
         <v>2</v>
@@ -918,7 +942,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B35" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -926,12 +950,12 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36">
         <f>SUM(C2:C35)</f>
-        <v>49.75</v>
+        <v>50.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
meeting notes with Christoph on prominent findings section
</commit_message>
<xml_diff>
--- a/New Features implementation plan-2020.xlsx
+++ b/New Features implementation plan-2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Igor Houwat - Branding - Alumni\Branding Tactics\Promotion\PRL Website\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B27FDE-1FA1-4018-B444-688BFEDD9DD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF9B256-FEE0-480E-AD22-5D5DBBAA68E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
   <si>
     <t>Feature</t>
   </si>
@@ -80,25 +80,13 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Touch base with Christoph</t>
-  </si>
-  <si>
     <t>Design timeline</t>
   </si>
   <si>
-    <t>Timeline copy</t>
-  </si>
-  <si>
-    <t>Timeline image assets</t>
-  </si>
-  <si>
     <t>Test on Mura</t>
   </si>
   <si>
     <t>Decide on content and website placement</t>
-  </si>
-  <si>
-    <t>Create page</t>
   </si>
   <si>
     <t>Determine pages that need to be changed</t>
@@ -198,7 +186,28 @@
     <t>Research format</t>
   </si>
   <si>
-    <t>A Zoom Timeline is too clunky</t>
+    <t>50 mins</t>
+  </si>
+  <si>
+    <t>A Zoom Timeline is too clunky. Form will be determined by the content.</t>
+  </si>
+  <si>
+    <t>Add to About page</t>
+  </si>
+  <si>
+    <t>40mins</t>
+  </si>
+  <si>
+    <t>Touched base with Christoph - will place on About Us page under Brief History</t>
+  </si>
+  <si>
+    <t>Rotating list through JS function</t>
+  </si>
+  <si>
+    <t>Write copy</t>
+  </si>
+  <si>
+    <t>Decide on image assets</t>
   </si>
 </sst>
 </file>
@@ -230,7 +239,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -245,7 +254,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -262,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -270,11 +285,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -581,7 +603,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -604,14 +626,14 @@
         <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
@@ -627,7 +649,7 @@
         <v>4.25</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -641,7 +663,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -651,16 +673,16 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -681,11 +703,11 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>33</v>
+      <c r="A8" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -694,12 +716,12 @@
         <v>0.5</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -721,7 +743,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -732,7 +754,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -741,11 +763,11 @@
         <v>0.5</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="2"/>
@@ -779,33 +801,36 @@
       <c r="B16" s="2"/>
     </row>
     <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B17" s="2" t="s">
-        <v>20</v>
+      <c r="B17" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="C17">
         <v>3</v>
       </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
       <c r="E17" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B18" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B18" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="C18">
         <v>1.25</v>
       </c>
-      <c r="D18">
-        <v>0.75</v>
+      <c r="D18" t="s">
+        <v>40</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B19" s="2" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="C19">
         <v>1.5</v>
@@ -813,23 +838,26 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B20" s="2" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B21" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C21">
-        <v>1.5</v>
+        <v>3</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B22" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -837,7 +865,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B23" s="2" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -852,7 +880,7 @@
     <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C25">
         <v>4</v>
@@ -861,7 +889,7 @@
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C26">
         <v>2</v>
@@ -870,7 +898,7 @@
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -879,7 +907,7 @@
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C28">
         <v>3</v>
@@ -888,7 +916,7 @@
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -897,36 +925,38 @@
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C30">
         <v>1.5</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C31">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+      <c r="A32" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="2"/>
-      <c r="E32" s="7" t="s">
-        <v>42</v>
+      <c r="B32" s="9"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="9" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="B33" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C33">
         <v>0.5</v>
@@ -934,7 +964,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B34" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C34">
         <v>2</v>
@@ -942,7 +972,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B35" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -950,12 +980,12 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36">
         <f>SUM(C2:C35)</f>
-        <v>50.5</v>
+        <v>50.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
testing Sciwheel API to access pub library
</commit_message>
<xml_diff>
--- a/New Features implementation plan-2020.xlsx
+++ b/New Features implementation plan-2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Igor Houwat - Branding - Alumni\Branding Tactics\Promotion\PRL Website\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF9B256-FEE0-480E-AD22-5D5DBBAA68E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76723ADC-ADF0-4346-856D-D8FE67CF3F30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>Feature</t>
   </si>
@@ -195,9 +195,6 @@
     <t>Add to About page</t>
   </si>
   <si>
-    <t>40mins</t>
-  </si>
-  <si>
     <t>Touched base with Christoph - will place on About Us page under Brief History</t>
   </si>
   <si>
@@ -208,6 +205,12 @@
   </si>
   <si>
     <t>Decide on image assets</t>
+  </si>
+  <si>
+    <t>1hr20mins</t>
+  </si>
+  <si>
+    <t>30mins</t>
   </si>
 </sst>
 </file>
@@ -602,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -805,13 +808,13 @@
         <v>17</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -830,7 +833,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B19" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19">
         <v>1.5</v>
@@ -838,7 +841,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B20" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20">
         <v>0.75</v>
@@ -851,8 +854,11 @@
       <c r="C21">
         <v>3</v>
       </c>
+      <c r="D21" t="s">
+        <v>48</v>
+      </c>
       <c r="E21" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -985,7 +991,7 @@
       <c r="B36" s="2"/>
       <c r="C36">
         <f>SUM(C2:C35)</f>
-        <v>50.75</v>
+        <v>51.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Write down thought process for Sciwheel api fetch
</commit_message>
<xml_diff>
--- a/New Features implementation plan-2020.xlsx
+++ b/New Features implementation plan-2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Igor Houwat - Branding - Alumni\Branding Tactics\Promotion\PRL Website\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76723ADC-ADF0-4346-856D-D8FE67CF3F30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CBA90D-2B32-4640-874D-F4E25FA2B68D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
   <si>
     <t>Feature</t>
   </si>
@@ -211,6 +211,12 @@
   </si>
   <si>
     <t>30mins</t>
+  </si>
+  <si>
+    <t>Test and Design API endpoints</t>
+  </si>
+  <si>
+    <t>Sciwheel API works well. EndNote does not</t>
   </si>
 </sst>
 </file>
@@ -327,8 +333,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{18181141-9763-4C4E-81E2-BD8C4A1BC2B5}" name="Table1" displayName="Table1" ref="A1:E36" totalsRowShown="0">
-  <autoFilter ref="A1:E36" xr:uid="{9D8E2DD3-3A32-40AB-A43D-21CD0663BC75}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{18181141-9763-4C4E-81E2-BD8C4A1BC2B5}" name="Table1" displayName="Table1" ref="A1:E37" totalsRowShown="0">
+  <autoFilter ref="A1:E37" xr:uid="{9D8E2DD3-3A32-40AB-A43D-21CD0663BC75}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{7F3EECCF-1821-47EC-B71B-035ADD8DACD4}" name="Feature"/>
     <tableColumn id="2" xr3:uid="{5FAB022F-5EFF-4925-8EBB-2E122BE73721}" name="Tasks" dataDxfId="1"/>
@@ -603,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -847,151 +853,165 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B21" s="2" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="C21">
         <v>3</v>
       </c>
-      <c r="D21" t="s">
-        <v>48</v>
+      <c r="D21">
+        <v>1.25</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B22" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B24" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C23">
+      <c r="C24">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="2"/>
-    </row>
-    <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="1"/>
-      <c r="B25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C28">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C30">
-        <v>1.5</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31">
+        <v>1.5</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="1"/>
+      <c r="B32" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C31">
+      <c r="C32">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="8" t="s">
+    <row r="33" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A33" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="9" t="s">
+      <c r="B33" s="9"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="B33" s="2" t="s">
+    <row r="34" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B34" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C33">
+      <c r="C34">
         <v>0.5</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B34" s="2" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B35" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C34">
+      <c r="C35">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B35" s="2" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B36" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C35">
+      <c r="C36">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="3" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B36" s="2"/>
-      <c r="C36">
-        <f>SUM(C2:C35)</f>
-        <v>51.75</v>
+      <c r="B37" s="2"/>
+      <c r="C37">
+        <f>SUM(C2:C36)</f>
+        <v>54.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sciwheel API fetches notes from database
</commit_message>
<xml_diff>
--- a/New Features implementation plan-2020.xlsx
+++ b/New Features implementation plan-2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Igor Houwat - Branding - Alumni\Branding Tactics\Promotion\PRL Website\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CBA90D-2B32-4640-874D-F4E25FA2B68D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484599A7-ADF7-47A0-A12F-F4018A77B1CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -216,7 +216,7 @@
     <t>Test and Design API endpoints</t>
   </si>
   <si>
-    <t>Sciwheel API works well. EndNote does not</t>
+    <t>Sciwheel API works well. EndNote doesn't work. Took much longer to implement than 3 hours…</t>
   </si>
 </sst>
 </file>
@@ -611,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -861,7 +861,7 @@
         <v>3</v>
       </c>
       <c r="D21">
-        <v>1.25</v>
+        <v>3</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
Sciwheel API - About page: added to db and increased randomness
</commit_message>
<xml_diff>
--- a/New Features implementation plan-2020.xlsx
+++ b/New Features implementation plan-2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Igor Houwat - Branding - Alumni\Branding Tactics\Promotion\PRL Website\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484599A7-ADF7-47A0-A12F-F4018A77B1CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F050E24F-273C-4027-B330-901BB76ABDEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
   <si>
     <t>Feature</t>
   </si>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t>Notes</t>
-  </si>
-  <si>
-    <t>Design timeline</t>
   </si>
   <si>
     <t>Test on Mura</t>
@@ -183,9 +180,6 @@
     <t>Prepare but postpone application. Due to COVID, MSU is asking for iages of people with PPE</t>
   </si>
   <si>
-    <t>Research format</t>
-  </si>
-  <si>
     <t>50 mins</t>
   </si>
   <si>
@@ -201,15 +195,9 @@
     <t>Rotating list through JS function</t>
   </si>
   <si>
-    <t>Write copy</t>
-  </si>
-  <si>
     <t>Decide on image assets</t>
   </si>
   <si>
-    <t>1hr20mins</t>
-  </si>
-  <si>
     <t>30mins</t>
   </si>
   <si>
@@ -217,6 +205,15 @@
   </si>
   <si>
     <t>Sciwheel API works well. EndNote doesn't work. Took much longer to implement than 3 hours…</t>
+  </si>
+  <si>
+    <t>Research display format</t>
+  </si>
+  <si>
+    <t>Write copy for achievements</t>
+  </si>
+  <si>
+    <t>Design list front-end</t>
   </si>
 </sst>
 </file>
@@ -286,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -308,11 +305,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -337,10 +340,10 @@
   <autoFilter ref="A1:E37" xr:uid="{9D8E2DD3-3A32-40AB-A43D-21CD0663BC75}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{7F3EECCF-1821-47EC-B71B-035ADD8DACD4}" name="Feature"/>
-    <tableColumn id="2" xr3:uid="{5FAB022F-5EFF-4925-8EBB-2E122BE73721}" name="Tasks" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{5FAB022F-5EFF-4925-8EBB-2E122BE73721}" name="Tasks" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{8FFB4A38-2812-4604-85EC-33574A58F8A9}" name="Time Cost (in hours)"/>
-    <tableColumn id="5" xr3:uid="{26D05208-6FB9-41CD-BB6D-843F20FE28C0}" name="Time spent"/>
-    <tableColumn id="4" xr3:uid="{93DF2C04-3550-4F5A-8C44-5008FCE2F361}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{26D05208-6FB9-41CD-BB6D-843F20FE28C0}" name="Time spent" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{93DF2C04-3550-4F5A-8C44-5008FCE2F361}" name="Notes" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -611,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -635,7 +638,7 @@
         <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>14</v>
@@ -646,6 +649,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
+      <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
@@ -654,11 +658,11 @@
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="5">
         <v>4.25</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -668,11 +672,11 @@
       <c r="C4">
         <v>5</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="5">
         <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -686,17 +690,17 @@
         <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="5">
         <v>4</v>
       </c>
     </row>
@@ -707,35 +711,35 @@
       <c r="C7">
         <v>0.5</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="5">
         <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="5">
         <v>0.5</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9">
         <v>3</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="5">
         <v>3</v>
       </c>
     </row>
@@ -746,33 +750,33 @@
       <c r="C10">
         <v>1</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="5">
         <v>0.5</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -780,6 +784,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="2"/>
+      <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B14" s="2" t="s">
@@ -788,7 +793,7 @@
       <c r="C14">
         <v>0.5</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="5">
         <v>0.25</v>
       </c>
     </row>
@@ -799,7 +804,7 @@
       <c r="C15">
         <v>0.25</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="5">
         <v>0.1</v>
       </c>
     </row>
@@ -808,166 +813,179 @@
         <v>6</v>
       </c>
       <c r="B16" s="2"/>
+      <c r="D16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B17" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17">
         <v>4</v>
       </c>
-      <c r="D17" t="s">
-        <v>47</v>
+      <c r="D17" s="5">
+        <v>2.5</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B18" s="10" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C18">
         <v>1.25</v>
       </c>
-      <c r="D18" t="s">
-        <v>40</v>
+      <c r="D18" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B19" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B19" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="C19">
         <v>1.5</v>
       </c>
+      <c r="D19" s="5"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B20" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C20">
         <v>0.75</v>
       </c>
+      <c r="D20" s="5"/>
     </row>
     <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B21" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C21">
         <v>3</v>
       </c>
-      <c r="D21">
-        <v>3</v>
+      <c r="D21" s="5">
+        <v>3.25</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B22" s="2" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="C22">
         <v>3</v>
       </c>
-      <c r="D22" t="s">
-        <v>48</v>
+      <c r="D22" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B23" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C23">
         <v>2</v>
       </c>
+      <c r="D23" s="5"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B24" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
+      <c r="D24" s="5"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="2"/>
+      <c r="D25" s="5"/>
     </row>
     <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C26">
         <v>4</v>
       </c>
+      <c r="D26" s="5"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C27">
         <v>2</v>
       </c>
+      <c r="D27" s="5"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
+      <c r="D28" s="5"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C29">
         <v>3</v>
       </c>
+      <c r="D29" s="5"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C30">
         <v>2</v>
       </c>
+      <c r="D30" s="5"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C31">
         <v>1.5</v>
       </c>
+      <c r="D31" s="5"/>
       <c r="E31" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="B32" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C32">
         <v>1</v>
       </c>
+      <c r="D32" s="5"/>
     </row>
     <row r="33" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="8" t="s">
@@ -975,44 +993,48 @@
       </c>
       <c r="B33" s="9"/>
       <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
+      <c r="D33" s="11"/>
       <c r="E33" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B34" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C34">
         <v>0.5</v>
       </c>
+      <c r="D34" s="5"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B35" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C35">
         <v>2</v>
       </c>
+      <c r="D35" s="5"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B36" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C36">
         <v>1</v>
       </c>
+      <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37">
         <f>SUM(C2:C36)</f>
         <v>54.75</v>
       </c>
+      <c r="D37" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
About page - important discoveries design prototype
</commit_message>
<xml_diff>
--- a/New Features implementation plan-2020.xlsx
+++ b/New Features implementation plan-2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Igor Houwat - Branding - Alumni\Branding Tactics\Promotion\PRL Website\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F050E24F-273C-4027-B330-901BB76ABDEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207727A0-5987-4558-B2D2-5743E9767E30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>Feature</t>
   </si>
@@ -56,9 +56,6 @@
     <t>Prominent findings page</t>
   </si>
   <si>
-    <t>For the public' page</t>
-  </si>
-  <si>
     <t>Images of People</t>
   </si>
   <si>
@@ -114,9 +111,6 @@
   </si>
   <si>
     <t>Publish</t>
-  </si>
-  <si>
-    <t>Time spent</t>
   </si>
   <si>
     <t>News story progress bar</t>
@@ -180,9 +174,6 @@
     <t>Prepare but postpone application. Due to COVID, MSU is asking for iages of people with PPE</t>
   </si>
   <si>
-    <t>50 mins</t>
-  </si>
-  <si>
     <t>A Zoom Timeline is too clunky. Form will be determined by the content.</t>
   </si>
   <si>
@@ -192,15 +183,9 @@
     <t>Touched base with Christoph - will place on About Us page under Brief History</t>
   </si>
   <si>
-    <t>Rotating list through JS function</t>
-  </si>
-  <si>
     <t>Decide on image assets</t>
   </si>
   <si>
-    <t>30mins</t>
-  </si>
-  <si>
     <t>Test and Design API endpoints</t>
   </si>
   <si>
@@ -214,6 +199,18 @@
   </si>
   <si>
     <t>Design list front-end</t>
+  </si>
+  <si>
+    <t>2hr 35 minutes</t>
+  </si>
+  <si>
+    <t>For the public page</t>
+  </si>
+  <si>
+    <t>Time spent (in hours)</t>
+  </si>
+  <si>
+    <t>Adobe XD mockup</t>
   </si>
 </sst>
 </file>
@@ -314,10 +311,10 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -342,8 +339,8 @@
     <tableColumn id="1" xr3:uid="{7F3EECCF-1821-47EC-B71B-035ADD8DACD4}" name="Feature"/>
     <tableColumn id="2" xr3:uid="{5FAB022F-5EFF-4925-8EBB-2E122BE73721}" name="Tasks" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{8FFB4A38-2812-4604-85EC-33574A58F8A9}" name="Time Cost (in hours)"/>
-    <tableColumn id="5" xr3:uid="{26D05208-6FB9-41CD-BB6D-843F20FE28C0}" name="Time spent" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{93DF2C04-3550-4F5A-8C44-5008FCE2F361}" name="Notes" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{26D05208-6FB9-41CD-BB6D-843F20FE28C0}" name="Time spent (in hours)" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{93DF2C04-3550-4F5A-8C44-5008FCE2F361}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -614,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -635,13 +632,13 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -653,7 +650,7 @@
     </row>
     <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -662,12 +659,12 @@
         <v>4.25</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>5</v>
@@ -676,12 +673,12 @@
         <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -690,12 +687,12 @@
         <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -706,7 +703,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7">
         <v>0.5</v>
@@ -717,10 +714,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -729,12 +726,12 @@
         <v>0.5</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -745,7 +742,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -756,7 +753,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -767,7 +764,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -776,7 +773,7 @@
         <v>0.5</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -816,14 +813,14 @@
       <c r="D16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B17" s="6" t="s">
-        <v>16</v>
+      <c r="B17" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D17" s="5">
-        <v>2.5</v>
+        <v>3.25</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>41</v>
@@ -831,67 +828,67 @@
     </row>
     <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B18" s="10" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C18">
         <v>1.25</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="5">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B19" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="2" t="s">
+    </row>
+    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B20" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20">
+        <v>1.5</v>
+      </c>
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B21" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B19" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19">
-        <v>1.5</v>
-      </c>
-      <c r="D19" s="5"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B20" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20">
+      <c r="C21">
         <v>0.75</v>
       </c>
-      <c r="D20" s="5"/>
-    </row>
-    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B21" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21">
-        <v>3</v>
-      </c>
-      <c r="D21" s="5">
-        <v>3.25</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>46</v>
-      </c>
+      <c r="D21" s="5"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B22" s="2" t="s">
-        <v>49</v>
+      <c r="B22" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="C22">
         <v>3</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>44</v>
+      <c r="D22" s="5">
+        <v>1</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B23" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -900,7 +897,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B24" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -909,7 +906,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="B25" s="2"/>
       <c r="D25" s="5"/>
@@ -917,7 +914,7 @@
     <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C26">
         <v>4</v>
@@ -927,7 +924,7 @@
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C27">
         <v>2</v>
@@ -937,7 +934,7 @@
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -947,7 +944,7 @@
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C29">
         <v>3</v>
@@ -957,7 +954,7 @@
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C30">
         <v>2</v>
@@ -967,20 +964,20 @@
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C31">
         <v>1.5</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="B32" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -989,18 +986,18 @@
     </row>
     <row r="33" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B33" s="9"/>
       <c r="C33" s="8"/>
       <c r="D33" s="11"/>
       <c r="E33" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B34" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C34">
         <v>0.5</v>
@@ -1009,7 +1006,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B35" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C35">
         <v>2</v>
@@ -1018,7 +1015,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B36" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -1027,7 +1024,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37">

</xml_diff>

<commit_message>
About page - impt. discoveries XD design
</commit_message>
<xml_diff>
--- a/New Features implementation plan-2020.xlsx
+++ b/New Features implementation plan-2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Igor Houwat - Branding - Alumni\Branding Tactics\Promotion\PRL Website\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207727A0-5987-4558-B2D2-5743E9767E30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C94CEE-4825-44B7-815F-16F2AE7EE90C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
   <si>
     <t>Feature</t>
   </si>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t>Adobe XD mockup</t>
+  </si>
+  <si>
+    <t>1hr 40 minutes</t>
   </si>
 </sst>
 </file>
@@ -280,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -303,6 +306,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -612,7 +618,7 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="D21" sqref="C21:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -867,10 +873,10 @@
       <c r="B21" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="4">
         <v>0.75</v>
       </c>
-      <c r="D21" s="5"/>
+      <c r="D21" s="12"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B22" s="6" t="s">
@@ -879,8 +885,8 @@
       <c r="C22">
         <v>3</v>
       </c>
-      <c r="D22" s="5">
-        <v>1</v>
+      <c r="D22" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
About page - impt. discoveries: finished design mockup
</commit_message>
<xml_diff>
--- a/New Features implementation plan-2020.xlsx
+++ b/New Features implementation plan-2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Igor Houwat - Branding - Alumni\Branding Tactics\Promotion\PRL Website\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C94CEE-4825-44B7-815F-16F2AE7EE90C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318FB215-04FE-447C-8C91-B02B037BA431}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>Feature</t>
   </si>
@@ -183,9 +183,6 @@
     <t>Touched base with Christoph - will place on About Us page under Brief History</t>
   </si>
   <si>
-    <t>Decide on image assets</t>
-  </si>
-  <si>
     <t>Test and Design API endpoints</t>
   </si>
   <si>
@@ -198,9 +195,6 @@
     <t>Write copy for achievements</t>
   </si>
   <si>
-    <t>Design list front-end</t>
-  </si>
-  <si>
     <t>2hr 35 minutes</t>
   </si>
   <si>
@@ -210,10 +204,13 @@
     <t>Time spent (in hours)</t>
   </si>
   <si>
-    <t>Adobe XD mockup</t>
-  </si>
-  <si>
-    <t>1hr 40 minutes</t>
+    <t>Decide on image asset</t>
+  </si>
+  <si>
+    <t>Adobe XD mockup complete</t>
+  </si>
+  <si>
+    <t>Design front-end</t>
   </si>
 </sst>
 </file>
@@ -283,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -302,14 +299,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -617,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D21" sqref="C21:D21"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -641,7 +639,7 @@
         <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>13</v>
@@ -819,8 +817,8 @@
       <c r="D16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B17" s="2" t="s">
-        <v>40</v>
+      <c r="B17" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="C17">
         <v>3</v>
@@ -829,12 +827,12 @@
         <v>3.25</v>
       </c>
       <c r="E17" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B18" s="13" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B18" s="10" t="s">
-        <v>42</v>
       </c>
       <c r="C18">
         <v>1.25</v>
@@ -847,49 +845,53 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="13" t="s">
         <v>15</v>
       </c>
       <c r="C19">
         <v>4</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B20" s="10" t="s">
-        <v>43</v>
+      <c r="B20" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="C20">
         <v>1.5</v>
       </c>
-      <c r="D20" s="5"/>
+      <c r="D20" s="5">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B21" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="4">
+      <c r="B21" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="11">
         <v>0.75</v>
       </c>
-      <c r="D21" s="12"/>
+      <c r="D21" s="12">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B22" s="6" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C22">
         <v>3</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>49</v>
+      <c r="D22" s="5">
+        <v>1.75</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -912,7 +914,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B25" s="2"/>
       <c r="D25" s="5"/>
@@ -996,7 +998,7 @@
       </c>
       <c r="B33" s="9"/>
       <c r="C33" s="8"/>
-      <c r="D33" s="11"/>
+      <c r="D33" s="10"/>
       <c r="E33" s="9" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
Abt page/impt. discoveries: implement front-end Mura design
</commit_message>
<xml_diff>
--- a/New Features implementation plan-2020.xlsx
+++ b/New Features implementation plan-2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Igor Houwat - Branding - Alumni\Branding Tactics\Promotion\PRL Website\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318FB215-04FE-447C-8C91-B02B037BA431}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA860D2-21D1-4AA2-A0D4-4125DB51753B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -207,10 +207,10 @@
     <t>Decide on image asset</t>
   </si>
   <si>
-    <t>Adobe XD mockup complete</t>
-  </si>
-  <si>
     <t>Design front-end</t>
+  </si>
+  <si>
+    <t>Adobe XD mockup complete; designing front-end straight in Mura</t>
   </si>
 </sst>
 </file>
@@ -615,7 +615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -880,18 +880,18 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B22" s="6" t="s">
-        <v>48</v>
+    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B22" s="13" t="s">
+        <v>47</v>
       </c>
       <c r="C22">
         <v>3</v>
       </c>
       <c r="D22" s="5">
-        <v>1.75</v>
+        <v>3</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Abt page/impt. discoveries: implement JS code
</commit_message>
<xml_diff>
--- a/New Features implementation plan-2020.xlsx
+++ b/New Features implementation plan-2020.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Igor Houwat - Branding - Alumni\Branding Tactics\Promotion\PRL Website\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA860D2-21D1-4AA2-A0D4-4125DB51753B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87191FEB-9C54-4CD9-B597-963D1BB1A8D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
   <si>
     <t>Feature</t>
   </si>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t>Adobe XD mockup complete; designing front-end straight in Mura</t>
+  </si>
+  <si>
+    <t>Fixed bugs, tested different browsers and devices</t>
   </si>
 </sst>
 </file>
@@ -616,7 +619,7 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -895,13 +898,18 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="13" t="s">
         <v>14</v>
       </c>
       <c r="C23">
         <v>2</v>
       </c>
-      <c r="D23" s="5"/>
+      <c r="D23" s="5">
+        <v>2.75</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B24" s="2" t="s">

</xml_diff>

<commit_message>
About page/impt. discoveries: content has gone live
</commit_message>
<xml_diff>
--- a/New Features implementation plan-2020.xlsx
+++ b/New Features implementation plan-2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Igor Houwat - Branding - Alumni\Branding Tactics\Promotion\PRL Website\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87191FEB-9C54-4CD9-B597-963D1BB1A8D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91B22A1-290D-4682-BBDA-885F4546739C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
   <si>
     <t>Feature</t>
   </si>
@@ -214,6 +214,12 @@
   </si>
   <si>
     <t>Fixed bugs, tested different browsers and devices</t>
+  </si>
+  <si>
+    <t>Share database with faculty for edits</t>
+  </si>
+  <si>
+    <t>Worked with Christoph to develop db content</t>
   </si>
 </sst>
 </file>
@@ -340,8 +346,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{18181141-9763-4C4E-81E2-BD8C4A1BC2B5}" name="Table1" displayName="Table1" ref="A1:E37" totalsRowShown="0">
-  <autoFilter ref="A1:E37" xr:uid="{9D8E2DD3-3A32-40AB-A43D-21CD0663BC75}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{18181141-9763-4C4E-81E2-BD8C4A1BC2B5}" name="Table1" displayName="Table1" ref="A1:E38" totalsRowShown="0">
+  <autoFilter ref="A1:E38" xr:uid="{9D8E2DD3-3A32-40AB-A43D-21CD0663BC75}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{7F3EECCF-1821-47EC-B71B-035ADD8DACD4}" name="Feature"/>
     <tableColumn id="2" xr3:uid="{5FAB022F-5EFF-4925-8EBB-2E122BE73721}" name="Tasks" dataDxfId="2"/>
@@ -616,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -862,14 +868,17 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="13" t="s">
         <v>42</v>
       </c>
       <c r="C20">
         <v>1.5</v>
       </c>
       <c r="D20" s="5">
-        <v>0.25</v>
+        <v>2</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -912,142 +921,153 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="13" t="s">
         <v>37</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
-      <c r="D24" s="5"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
+      <c r="D24" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B25" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" s="5"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="D25" s="5"/>
-    </row>
-    <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="1"/>
-      <c r="B26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26">
-        <v>4</v>
-      </c>
+      <c r="B26" s="2"/>
       <c r="D26" s="5"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D27" s="5"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D28" s="5"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C29">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D29" s="5"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D30" s="5"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="2" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C31">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="D31" s="5"/>
-      <c r="E31" s="2" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="B32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32">
+        <v>1.5</v>
+      </c>
+      <c r="D32" s="5"/>
+      <c r="E32" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="1"/>
+      <c r="B33" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C32">
+      <c r="C33">
         <v>1</v>
       </c>
-      <c r="D32" s="5"/>
-    </row>
-    <row r="33" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A33" s="8" t="s">
+      <c r="D33" s="5"/>
+    </row>
+    <row r="34" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A34" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="9" t="s">
+      <c r="B34" s="9"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B34" s="2" t="s">
+    <row r="35" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B35" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C34">
+      <c r="C35">
         <v>0.5</v>
-      </c>
-      <c r="D34" s="5"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B35" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C35">
-        <v>2</v>
       </c>
       <c r="D35" s="5"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36" s="5"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B37" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C36">
+      <c r="C37">
         <v>1</v>
       </c>
-      <c r="D36" s="5"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="3" t="s">
+      <c r="D37" s="5"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="2"/>
-      <c r="C37">
-        <f>SUM(C2:C36)</f>
-        <v>54.75</v>
-      </c>
-      <c r="D37" s="5"/>
+      <c r="B38" s="2"/>
+      <c r="C38">
+        <f>SUM(C2:C37)</f>
+        <v>55.75</v>
+      </c>
+      <c r="D38" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
shortened progress bar height
</commit_message>
<xml_diff>
--- a/New Features implementation plan-2020.xlsx
+++ b/New Features implementation plan-2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Igor Houwat - Branding - Alumni\Branding Tactics\Promotion\PRL Website\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91B22A1-290D-4682-BBDA-885F4546739C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F03BAF2-8DE3-43F3-9B40-D0F35262C31A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>Create copy</t>
-  </si>
-  <si>
-    <t>Copy revisions</t>
   </si>
   <si>
     <t>Codepen mockup</t>
@@ -171,9 +168,6 @@
     <t>Includes cross browser testing</t>
   </si>
   <si>
-    <t>Prepare but postpone application. Due to COVID, MSU is asking for iages of people with PPE</t>
-  </si>
-  <si>
     <t>A Zoom Timeline is too clunky. Form will be determined by the content.</t>
   </si>
   <si>
@@ -195,9 +189,6 @@
     <t>Write copy for achievements</t>
   </si>
   <si>
-    <t>2hr 35 minutes</t>
-  </si>
-  <si>
     <t>For the public page</t>
   </si>
   <si>
@@ -220,6 +211,15 @@
   </si>
   <si>
     <t>Worked with Christoph to develop db content</t>
+  </si>
+  <si>
+    <t>Exported spreadsheet of entries and edited for faculty to explore</t>
+  </si>
+  <si>
+    <t>Copy revisions w/faculty</t>
+  </si>
+  <si>
+    <t>Prepare but postpone application. Due to COVID, MSU is asking for images of people with PPE</t>
   </si>
 </sst>
 </file>
@@ -289,19 +289,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -315,9 +311,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,8 +621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -648,18 +645,18 @@
         <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="D2" s="5"/>
+      <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
@@ -668,11 +665,11 @@
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>4.25</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -682,11 +679,11 @@
       <c r="C4">
         <v>5</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -696,11 +693,11 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -710,7 +707,7 @@
       <c r="C6">
         <v>2</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>4</v>
       </c>
     </row>
@@ -721,35 +718,35 @@
       <c r="C7">
         <v>0.5</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>0.5</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9">
         <v>3</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>3</v>
       </c>
     </row>
@@ -760,7 +757,7 @@
       <c r="C10">
         <v>1</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>0</v>
       </c>
     </row>
@@ -771,30 +768,30 @@
       <c r="C11">
         <v>2</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>0.5</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="2"/>
-      <c r="D13" s="5"/>
+      <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B14" s="2" t="s">
@@ -803,7 +800,7 @@
       <c r="C14">
         <v>0.5</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>0.25</v>
       </c>
     </row>
@@ -814,138 +811,143 @@
       <c r="C15">
         <v>0.25</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>0.1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="2"/>
-      <c r="D16" s="5"/>
+      <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B17" s="13" t="s">
-        <v>39</v>
+      <c r="B17" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="C17">
         <v>3</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="4">
         <v>3.25</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B18" s="13" t="s">
-        <v>41</v>
+      <c r="B18" s="11" t="s">
+        <v>39</v>
       </c>
       <c r="C18">
         <v>1.25</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="4">
         <v>1</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="11" t="s">
         <v>15</v>
       </c>
       <c r="C19">
         <v>4</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>43</v>
+      <c r="D19" s="4">
+        <v>2.5</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B20" s="13" t="s">
-        <v>42</v>
+      <c r="B20" s="11" t="s">
+        <v>40</v>
       </c>
       <c r="C20">
         <v>1.5</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="4">
         <v>2</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B21" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" s="11">
+      <c r="B21" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="9">
         <v>0.75</v>
       </c>
-      <c r="D21" s="12">
+      <c r="D21" s="10">
         <v>0.75</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B22" s="13" t="s">
-        <v>47</v>
+      <c r="B22" s="11" t="s">
+        <v>44</v>
       </c>
       <c r="C22">
         <v>3</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="4">
         <v>3</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="11" t="s">
         <v>14</v>
       </c>
       <c r="C23">
         <v>2</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="4">
         <v>2.75</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B24" s="13" t="s">
-        <v>37</v>
+      <c r="B24" s="11" t="s">
+        <v>35</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B25" s="6" t="s">
-        <v>50</v>
+      <c r="B25" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
-      <c r="D25" s="5"/>
+      <c r="D25" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
-        <v>44</v>
+      <c r="A26" s="12" t="s">
+        <v>41</v>
       </c>
       <c r="B26" s="2"/>
-      <c r="D26" s="5"/>
+      <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
@@ -955,7 +957,7 @@
       <c r="C27">
         <v>4</v>
       </c>
-      <c r="D27" s="5"/>
+      <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
@@ -963,19 +965,19 @@
         <v>21</v>
       </c>
       <c r="C28">
-        <v>2</v>
-      </c>
-      <c r="D28" s="5"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="2" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
-      <c r="D29" s="5"/>
+      <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
@@ -985,17 +987,17 @@
       <c r="C30">
         <v>3</v>
       </c>
-      <c r="D30" s="5"/>
+      <c r="D30" s="4"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C31">
         <v>2</v>
       </c>
-      <c r="D31" s="5"/>
+      <c r="D31" s="4"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
@@ -1005,30 +1007,30 @@
       <c r="C32">
         <v>1.5</v>
       </c>
-      <c r="D32" s="5"/>
+      <c r="D32" s="4"/>
       <c r="E32" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
       <c r="B33" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C33">
         <v>1</v>
       </c>
-      <c r="D33" s="5"/>
+      <c r="D33" s="4"/>
     </row>
     <row r="34" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="9"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="9" t="s">
-        <v>35</v>
+      <c r="B34" s="7"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="7" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1038,7 +1040,7 @@
       <c r="C35">
         <v>0.5</v>
       </c>
-      <c r="D35" s="5"/>
+      <c r="D35" s="4"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B36" s="2" t="s">
@@ -1047,7 +1049,7 @@
       <c r="C36">
         <v>2</v>
       </c>
-      <c r="D36" s="5"/>
+      <c r="D36" s="4"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B37" s="2" t="s">
@@ -1056,7 +1058,7 @@
       <c r="C37">
         <v>1</v>
       </c>
-      <c r="D37" s="5"/>
+      <c r="D37" s="4"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
@@ -1065,9 +1067,12 @@
       <c r="B38" s="2"/>
       <c r="C38">
         <f>SUM(C2:C37)</f>
-        <v>55.75</v>
-      </c>
-      <c r="D38" s="5"/>
+        <v>56.75</v>
+      </c>
+      <c r="D38" s="4">
+        <f>SUM(D2:D37)</f>
+        <v>42.85</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
'for the public' page - began research
</commit_message>
<xml_diff>
--- a/New Features implementation plan-2020.xlsx
+++ b/New Features implementation plan-2020.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Igor Houwat - Branding - Alumni\Branding Tactics\Promotion\PRL Website\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F03BAF2-8DE3-43F3-9B40-D0F35262C31A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E82DD0-85D1-499B-944D-2FDF4BCBB43F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
   <si>
     <t>Feature</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>Prepare but postpone application. Due to COVID, MSU is asking for images of people with PPE</t>
+  </si>
+  <si>
+    <t>Collect/produce visual assets</t>
   </si>
 </sst>
 </file>
@@ -314,7 +317,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -343,8 +348,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{18181141-9763-4C4E-81E2-BD8C4A1BC2B5}" name="Table1" displayName="Table1" ref="A1:E38" totalsRowShown="0">
-  <autoFilter ref="A1:E38" xr:uid="{9D8E2DD3-3A32-40AB-A43D-21CD0663BC75}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{18181141-9763-4C4E-81E2-BD8C4A1BC2B5}" name="Table1" displayName="Table1" ref="A1:E39" totalsRowShown="0">
+  <autoFilter ref="A1:E39" xr:uid="{9D8E2DD3-3A32-40AB-A43D-21CD0663BC75}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{7F3EECCF-1821-47EC-B71B-035ADD8DACD4}" name="Feature"/>
     <tableColumn id="2" xr3:uid="{5FAB022F-5EFF-4925-8EBB-2E122BE73721}" name="Tasks" dataDxfId="2"/>
@@ -619,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -812,7 +817,7 @@
         <v>0.25</v>
       </c>
       <c r="D15" s="4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -943,135 +948,147 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B26" s="2"/>
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
-      <c r="B27" s="2" t="s">
-        <v>20</v>
+      <c r="B27" s="12" t="s">
+        <v>8</v>
       </c>
       <c r="C27">
-        <v>4</v>
-      </c>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2.5</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C28">
         <v>3</v>
       </c>
       <c r="D28" s="4"/>
     </row>
-    <row r="29" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="2" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D29" s="4"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="2" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D30" s="4"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="2" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="C31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D31" s="4"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="B32" s="2" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C32">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="D32" s="4"/>
-      <c r="E32" s="2" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
       <c r="B33" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33">
+        <v>1.5</v>
+      </c>
+      <c r="D33" s="4"/>
+      <c r="E33" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="1"/>
+      <c r="B34" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C33">
+      <c r="C34">
         <v>1</v>
       </c>
-      <c r="D33" s="4"/>
-    </row>
-    <row r="34" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="6" t="s">
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A35" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="7"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="7" t="s">
+      <c r="B35" s="7"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B35" s="2" t="s">
+    <row r="36" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B36" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C35">
+      <c r="C36">
         <v>0.5</v>
-      </c>
-      <c r="D35" s="4"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C36">
-        <v>2</v>
       </c>
       <c r="D36" s="4"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B37" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B38" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C37">
+      <c r="C38">
         <v>1</v>
       </c>
-      <c r="D37" s="4"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="3" t="s">
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B38" s="2"/>
-      <c r="C38">
-        <f>SUM(C2:C37)</f>
-        <v>56.75</v>
-      </c>
-      <c r="D38" s="4">
-        <f>SUM(D2:D37)</f>
-        <v>42.85</v>
+      <c r="B39" s="2"/>
+      <c r="C39">
+        <f>SUM(C2:C38)</f>
+        <v>58.25</v>
+      </c>
+      <c r="D39" s="4">
+        <f>SUM(D2:D38)</f>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>